<commit_message>
Pohled fakulty: Zatím všechno ok
Úspěch při generování tabulek, bombátoru nic nevadí
Potenciální problém: Vypnutý strict mode při castění, možná ztráta dat

Another happy landing
</commit_message>
<xml_diff>
--- a/results/cvicici_bez_cviceni.xlsx
+++ b/results/cvicici_bez_cviceni.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="191">
   <si>
     <t>nazev</t>
   </si>
@@ -25,91 +25,569 @@
     <t>cviciciUcitIdno</t>
   </si>
   <si>
-    <t>Teoretická informatika a matematika</t>
+    <t>Fyzika pevných látek I</t>
+  </si>
+  <si>
+    <t>Demografie</t>
+  </si>
+  <si>
+    <t>Geometrie</t>
+  </si>
+  <si>
+    <t>Fyziologie a mol. bio. eukar. buňky I</t>
+  </si>
+  <si>
+    <t>Fyziologie živočichů a člověka</t>
+  </si>
+  <si>
+    <t>Proseminář řešení fyzikálních úloh</t>
+  </si>
+  <si>
+    <t>Fyzikální praktikum C</t>
+  </si>
+  <si>
+    <t>Proseminář řešení fyzikálních úloh A ZŠ</t>
+  </si>
+  <si>
+    <t>Průběžná pedagogická praxe ZŠ</t>
+  </si>
+  <si>
+    <t>Didaktická a laboratorní technika</t>
+  </si>
+  <si>
+    <t>Souvislá pedagogická praxe II - ZŠ</t>
+  </si>
+  <si>
+    <t>Exkurze</t>
+  </si>
+  <si>
+    <t>Matematický proseminář</t>
+  </si>
+  <si>
+    <t>Souhrnný seminář - počítačové modelování</t>
+  </si>
+  <si>
+    <t>Kvantová mechanika</t>
+  </si>
+  <si>
+    <t>Teorie elektromagnetického pole</t>
+  </si>
+  <si>
+    <t>Kvantová fyzika II</t>
+  </si>
+  <si>
+    <t>Seminář katedry II</t>
+  </si>
+  <si>
+    <t>PVK - Vyb.partie z teoretické fyziky II</t>
+  </si>
+  <si>
+    <t>Fyzika I</t>
+  </si>
+  <si>
+    <t>Kvantová fyzika</t>
+  </si>
+  <si>
+    <t>PVK - Vyb.partie z teoretické fyziky I</t>
+  </si>
+  <si>
+    <t>Vybrané partie z teorie elektromag. pole</t>
+  </si>
+  <si>
+    <t>Vybrané partie z teoretické fyziky I</t>
+  </si>
+  <si>
+    <t>Seminář katedry I</t>
+  </si>
+  <si>
+    <t>Seminář katedry</t>
+  </si>
+  <si>
+    <t>Potenciál kulturní krajiny a GIS</t>
+  </si>
+  <si>
+    <t>Metody geografického výzkumu krajiny</t>
+  </si>
+  <si>
+    <t>Dějiny chemie</t>
+  </si>
+  <si>
+    <t>Didaktika chemie II - SŠ</t>
+  </si>
+  <si>
+    <t>Vybrané matematické metody ve fyzice</t>
+  </si>
+  <si>
+    <t>Experimentální využití elmg. vln F</t>
+  </si>
+  <si>
+    <t>VK- Praktikum mikrovlnné techniky D</t>
+  </si>
+  <si>
+    <t>Experimentální využití elmg. vln B</t>
+  </si>
+  <si>
+    <t>Řešení obvodu RLC</t>
+  </si>
+  <si>
+    <t>Počítačové modelování I</t>
+  </si>
+  <si>
+    <t>PVK - Hromadné zpracování dat</t>
+  </si>
+  <si>
+    <t>Systém kvality a vyhodnocování dat</t>
+  </si>
+  <si>
+    <t>Počítač. modelování - spojité modelování</t>
+  </si>
+  <si>
+    <t>Základy financí</t>
+  </si>
+  <si>
+    <t>Finanční analýza</t>
+  </si>
+  <si>
+    <t>Somatologie</t>
+  </si>
+  <si>
+    <t>Ekofyziologie</t>
+  </si>
+  <si>
+    <t>Biologie parazitů</t>
+  </si>
+  <si>
+    <t>Obecná zoologie</t>
+  </si>
+  <si>
+    <t>Met. analýz mat. 
+využ. el. mikroskopie</t>
+  </si>
+  <si>
+    <t>Metody analýz materiálů</t>
+  </si>
+  <si>
+    <t>Algologie</t>
+  </si>
+  <si>
+    <t>Didaktika geografie I</t>
+  </si>
+  <si>
+    <t>Labor. Techniq. in Mol. and Cell Biology</t>
+  </si>
+  <si>
+    <t>VK-Česká republika a EU</t>
+  </si>
+  <si>
+    <t>VK - Konverzace němčiny pro geografy</t>
+  </si>
+  <si>
+    <t>Medicína katastrof</t>
+  </si>
+  <si>
+    <t>Technologie ochrany životního prostředí</t>
+  </si>
+  <si>
+    <t>Ekotoxikologie</t>
+  </si>
+  <si>
+    <t>Toxikologie rostl. a živočišných toxinů</t>
   </si>
   <si>
     <t>Počítačová kriminalita</t>
   </si>
   <si>
-    <t>Modelování podnikových procesů</t>
+    <t>Welfare Assessment of zoo animals</t>
+  </si>
+  <si>
+    <t>Preparace a konzervování přírodnin II</t>
+  </si>
+  <si>
+    <t>Funkce a struktura buněčných membrán</t>
+  </si>
+  <si>
+    <t>Základy bioinženýrství</t>
   </si>
   <si>
     <t>Počítačové sítě a protokoly</t>
   </si>
   <si>
+    <t>Matematika I</t>
+  </si>
+  <si>
+    <t>Neziskový sektor a regionální rozvoj</t>
+  </si>
+  <si>
+    <t>Explantátové kultury rostlin I</t>
+  </si>
+  <si>
+    <t>Právní aspekty vzdělávání a předpisy</t>
+  </si>
+  <si>
     <t>Information Security</t>
   </si>
   <si>
     <t>Mikroprocesory a senzory v praxi II</t>
   </si>
   <si>
-    <t>Mikroprocesory a senzory v praxi I</t>
-  </si>
-  <si>
     <t>Automatické řízení</t>
   </si>
   <si>
-    <t>Analogová elektronika</t>
+    <t>Životní prostředí a udržitelný rozvoj</t>
+  </si>
+  <si>
+    <t>Terénní cvičení ze SG</t>
+  </si>
+  <si>
+    <t>English for Science</t>
+  </si>
+  <si>
+    <t>Zoologické terénní cvičení</t>
+  </si>
+  <si>
+    <t>Srovnávací anatom. a morfol. obratlovců</t>
+  </si>
+  <si>
+    <t>Ornitologie</t>
+  </si>
+  <si>
+    <t>Odběr, příprava a analýza vzorků</t>
+  </si>
+  <si>
+    <t>Přípr. a využití nanovlákenných struktur</t>
+  </si>
+  <si>
+    <t>Souvislá pedagogická praxe I - SŠ</t>
+  </si>
+  <si>
+    <t>Doučování</t>
+  </si>
+  <si>
+    <t>Didaktika biologie II</t>
+  </si>
+  <si>
+    <t>Didaktika biologie I</t>
+  </si>
+  <si>
+    <t>Souvislá pedagogická praxe II - SŠ</t>
+  </si>
+  <si>
+    <t>Kompozity nanočástic kovů a jejich oxidů</t>
+  </si>
+  <si>
+    <t>Apl. biologie prokaryot. a eukaryot. m.</t>
   </si>
   <si>
     <t>Python and R for Data Science</t>
   </si>
   <si>
+    <t>Algoritmizace a programování I</t>
+  </si>
+  <si>
     <t>Algoritmizace a programování II</t>
   </si>
   <si>
-    <t>Algoritmizace a programování I</t>
-  </si>
-  <si>
     <t>Objektově orientované návrhové vzory</t>
   </si>
   <si>
-    <t>YTIM</t>
+    <t>K839</t>
+  </si>
+  <si>
+    <t>FDEMO</t>
+  </si>
+  <si>
+    <t>5DEMO</t>
+  </si>
+  <si>
+    <t>P335</t>
+  </si>
+  <si>
+    <t>N016</t>
+  </si>
+  <si>
+    <t>KB502</t>
+  </si>
+  <si>
+    <t>PB502</t>
+  </si>
+  <si>
+    <t>K622</t>
+  </si>
+  <si>
+    <t>K521</t>
+  </si>
+  <si>
+    <t>P736</t>
+  </si>
+  <si>
+    <t>P732</t>
+  </si>
+  <si>
+    <t>PA31</t>
+  </si>
+  <si>
+    <t>KA35</t>
+  </si>
+  <si>
+    <t>P841</t>
+  </si>
+  <si>
+    <t>P365</t>
+  </si>
+  <si>
+    <t>KSPM</t>
+  </si>
+  <si>
+    <t>KM</t>
+  </si>
+  <si>
+    <t>TEP</t>
+  </si>
+  <si>
+    <t>P607</t>
+  </si>
+  <si>
+    <t>PA52</t>
+  </si>
+  <si>
+    <t>K522</t>
+  </si>
+  <si>
+    <t>K222</t>
+  </si>
+  <si>
+    <t>SPM</t>
+  </si>
+  <si>
+    <t>K724</t>
+  </si>
+  <si>
+    <t>KKM</t>
+  </si>
+  <si>
+    <t>K422</t>
+  </si>
+  <si>
+    <t>P737</t>
+  </si>
+  <si>
+    <t>PD203</t>
+  </si>
+  <si>
+    <t>P938</t>
+  </si>
+  <si>
+    <t>P952</t>
+  </si>
+  <si>
+    <t>P602</t>
+  </si>
+  <si>
+    <t>M214</t>
+  </si>
+  <si>
+    <t>M409</t>
+  </si>
+  <si>
+    <t>KN16</t>
+  </si>
+  <si>
+    <t>KN22</t>
+  </si>
+  <si>
+    <t>0212</t>
+  </si>
+  <si>
+    <t>0237</t>
+  </si>
+  <si>
+    <t>0211</t>
+  </si>
+  <si>
+    <t>0218</t>
+  </si>
+  <si>
+    <t>0214</t>
+  </si>
+  <si>
+    <t>K107</t>
+  </si>
+  <si>
+    <t>P406</t>
+  </si>
+  <si>
+    <t>N111</t>
+  </si>
+  <si>
+    <t>P366</t>
+  </si>
+  <si>
+    <t>ZFIN</t>
+  </si>
+  <si>
+    <t>FINA</t>
+  </si>
+  <si>
+    <t>BK423</t>
+  </si>
+  <si>
+    <t>N051</t>
+  </si>
+  <si>
+    <t>N032</t>
+  </si>
+  <si>
+    <t>K110</t>
+  </si>
+  <si>
+    <t>BP423</t>
+  </si>
+  <si>
+    <t>AP03</t>
+  </si>
+  <si>
+    <t>AP05</t>
+  </si>
+  <si>
+    <t>N036</t>
+  </si>
+  <si>
+    <t>N001</t>
+  </si>
+  <si>
+    <t>E121</t>
+  </si>
+  <si>
+    <t>0116</t>
+  </si>
+  <si>
+    <t>0130</t>
+  </si>
+  <si>
+    <t>P518</t>
+  </si>
+  <si>
+    <t>P414</t>
+  </si>
+  <si>
+    <t>N109</t>
+  </si>
+  <si>
+    <t>P534</t>
   </si>
   <si>
     <t>0141</t>
   </si>
   <si>
-    <t>0160</t>
+    <t>E133</t>
+  </si>
+  <si>
+    <t>P416</t>
+  </si>
+  <si>
+    <t>0088</t>
+  </si>
+  <si>
+    <t>0090</t>
   </si>
   <si>
     <t>PSP</t>
   </si>
   <si>
+    <t>P106</t>
+  </si>
+  <si>
+    <t>0150</t>
+  </si>
+  <si>
+    <t>N049</t>
+  </si>
+  <si>
+    <t>N005</t>
+  </si>
+  <si>
+    <t>KN46</t>
+  </si>
+  <si>
     <t>0177</t>
   </si>
   <si>
     <t>0171</t>
   </si>
   <si>
-    <t>0164</t>
-  </si>
-  <si>
     <t>AUC</t>
   </si>
   <si>
-    <t>ANE</t>
-  </si>
-  <si>
-    <t>KANE</t>
-  </si>
-  <si>
-    <t>KAEL</t>
+    <t>P861</t>
+  </si>
+  <si>
+    <t>P839</t>
+  </si>
+  <si>
+    <t>BK401</t>
+  </si>
+  <si>
+    <t>M312</t>
+  </si>
+  <si>
+    <t>E403</t>
+  </si>
+  <si>
+    <t>B401</t>
+  </si>
+  <si>
+    <t>KB427</t>
+  </si>
+  <si>
+    <t>N060</t>
+  </si>
+  <si>
+    <t>PB427</t>
+  </si>
+  <si>
+    <t>MA205</t>
+  </si>
+  <si>
+    <t>N112</t>
+  </si>
+  <si>
+    <t>PD55</t>
+  </si>
+  <si>
+    <t>P707A</t>
+  </si>
+  <si>
+    <t>DOUC</t>
+  </si>
+  <si>
+    <t>P208</t>
+  </si>
+  <si>
+    <t>P108</t>
+  </si>
+  <si>
+    <t>P707B</t>
+  </si>
+  <si>
+    <t>PD12</t>
+  </si>
+  <si>
+    <t>ME301</t>
   </si>
   <si>
     <t>EPYR</t>
   </si>
   <si>
+    <t>APR1</t>
+  </si>
+  <si>
     <t>APR2</t>
   </si>
   <si>
-    <t>APR1</t>
+    <t>KOONV</t>
   </si>
   <si>
     <t>OONV</t>
-  </si>
-  <si>
-    <t>KOONV</t>
   </si>
 </sst>
 </file>
@@ -171,8 +649,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Frame0" displayName="Frame0" ref="A1:C18" totalsRowShown="0">
-  <autoFilter ref="A1:C18"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Frame0" displayName="Frame0" ref="A1:C107" totalsRowShown="0">
+  <autoFilter ref="A1:C107"/>
   <tableColumns count="3">
     <tableColumn id="1" name="nazev" dataDxfId="0"/>
     <tableColumn id="2" name="zkratka" dataDxfId="0"/>
@@ -467,7 +945,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C107"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -489,10 +967,10 @@
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>16</v>
+        <v>91</v>
       </c>
       <c r="C2" s="2">
-        <v>3188</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -500,98 +978,98 @@
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>17</v>
+        <v>92</v>
       </c>
       <c r="C3" s="2">
-        <v>3458</v>
+        <v>130</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>18</v>
+        <v>93</v>
       </c>
       <c r="C4" s="2">
-        <v>4190</v>
+        <v>130</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>19</v>
+        <v>94</v>
       </c>
       <c r="C5" s="2">
-        <v>4195</v>
+        <v>269</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>20</v>
+        <v>95</v>
       </c>
       <c r="C6" s="2">
-        <v>4685</v>
+        <v>281</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>21</v>
+        <v>96</v>
       </c>
       <c r="C7" s="2">
-        <v>4746</v>
+        <v>281</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>22</v>
+        <v>97</v>
       </c>
       <c r="C8" s="2">
-        <v>4746</v>
+        <v>281</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>23</v>
+        <v>98</v>
       </c>
       <c r="C9" s="2">
-        <v>5039</v>
+        <v>302</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="1" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>16</v>
+        <v>99</v>
       </c>
       <c r="C10" s="2">
-        <v>5205</v>
+        <v>302</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>24</v>
+        <v>100</v>
       </c>
       <c r="C11" s="2">
-        <v>5232</v>
+        <v>302</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -599,75 +1077,1054 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>25</v>
+        <v>101</v>
       </c>
       <c r="C12" s="2">
-        <v>5232</v>
+        <v>302</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>26</v>
+        <v>102</v>
       </c>
       <c r="C13" s="2">
-        <v>5232</v>
+        <v>302</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>27</v>
+        <v>103</v>
       </c>
       <c r="C14" s="2">
-        <v>8514</v>
+        <v>302</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>28</v>
+        <v>104</v>
       </c>
       <c r="C15" s="2">
-        <v>8514</v>
+        <v>302</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>29</v>
+        <v>105</v>
       </c>
       <c r="C16" s="2">
-        <v>8514</v>
+        <v>306</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>30</v>
+        <v>106</v>
       </c>
       <c r="C17" s="2">
-        <v>8753</v>
+        <v>307</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C18" s="2">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C19" s="2">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C20" s="2">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C21" s="2">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C22" s="2">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C23" s="2">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C24" s="2">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C25" s="2">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C26" s="2">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C27" s="2">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C28" s="2">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C29" s="2">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C30" s="2">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C31" s="2">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C32" s="2">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C33" s="2">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C34" s="2">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C18" s="2">
+      <c r="B35" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C35" s="2">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C36" s="2">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C37" s="2">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C38" s="2">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C39" s="2">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C40" s="2">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C41" s="2">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C42" s="2">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C43" s="2">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C44" s="2">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C45" s="2">
+        <v>816</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C46" s="2">
+        <v>929</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C47" s="2">
+        <v>929</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C48" s="2">
+        <v>1383</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C49" s="2">
+        <v>1546</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C50" s="2">
+        <v>1546</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C51" s="2">
+        <v>1546</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C52" s="2">
+        <v>1546</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C53" s="2">
+        <v>1546</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C54" s="2">
+        <v>1590</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C55" s="2">
+        <v>1590</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C56" s="2">
+        <v>1999</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="C57" s="2">
+        <v>2232</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C58" s="2">
+        <v>2441</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="A59" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C59" s="2">
+        <v>2758</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="A60" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C60" s="2">
+        <v>2812</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="A61" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C61" s="2">
+        <v>3066</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
+      <c r="A62" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C62" s="2">
+        <v>3175</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
+      <c r="A63" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C63" s="2">
+        <v>3176</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
+      <c r="A64" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C64" s="2">
+        <v>3176</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
+      <c r="A65" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C65" s="2">
+        <v>3458</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
+      <c r="A66" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C66" s="2">
+        <v>3796</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
+      <c r="A67" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C67" s="2">
+        <v>3797</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C68" s="2">
+        <v>3798</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="A69" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C69" s="2">
+        <v>4175</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
+      <c r="A70" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C70" s="2">
+        <v>4177</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3">
+      <c r="A71" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C71" s="2">
+        <v>4195</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
+      <c r="A72" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C72" s="2">
+        <v>4208</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
+      <c r="A73" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="C73" s="2">
+        <v>4221</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3">
+      <c r="A74" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="C74" s="2">
+        <v>4227</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3">
+      <c r="A75" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C75" s="2">
+        <v>4390</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3">
+      <c r="A76" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C76" s="2">
+        <v>4581</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3">
+      <c r="A77" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="C77" s="2">
+        <v>4581</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3">
+      <c r="A78" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C78" s="2">
+        <v>4685</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3">
+      <c r="A79" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C79" s="2">
+        <v>4746</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3">
+      <c r="A80" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C80" s="2">
+        <v>5039</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3">
+      <c r="A81" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C81" s="2">
+        <v>5201</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3">
+      <c r="A82" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C82" s="2">
+        <v>5201</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3">
+      <c r="A83" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="C83" s="2">
+        <v>5240</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3">
+      <c r="A84" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C84" s="2">
+        <v>5240</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3">
+      <c r="A85" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="C85" s="2">
+        <v>5240</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3">
+      <c r="A86" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="C86" s="2">
+        <v>5240</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3">
+      <c r="A87" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C87" s="2">
+        <v>5472</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3">
+      <c r="A88" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="C88" s="2">
+        <v>5472</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3">
+      <c r="A89" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C89" s="2">
+        <v>5472</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3">
+      <c r="A90" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="C90" s="2">
+        <v>5472</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3">
+      <c r="A91" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C91" s="2">
+        <v>6120</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3">
+      <c r="A92" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="C92" s="2">
+        <v>7416</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3">
+      <c r="A93" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C93" s="2">
+        <v>7805</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3">
+      <c r="A94" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C94" s="2">
+        <v>8021</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3">
+      <c r="A95" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="C95" s="2">
+        <v>8021</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3">
+      <c r="A96" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="C96" s="2">
+        <v>8021</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3">
+      <c r="A97" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C97" s="2">
+        <v>8021</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3">
+      <c r="A98" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="C98" s="2">
+        <v>8021</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3">
+      <c r="A99" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C99" s="2">
+        <v>8074</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3">
+      <c r="A100" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="C100" s="2">
+        <v>8154</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3">
+      <c r="A101" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C101" s="2">
+        <v>8310</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3">
+      <c r="A102" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C102" s="2">
+        <v>8310</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3">
+      <c r="A103" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="C103" s="2">
+        <v>8514</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3">
+      <c r="A104" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="C104" s="2">
+        <v>8514</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3">
+      <c r="A105" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="C105" s="2">
+        <v>8514</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3">
+      <c r="A106" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="C106" s="2">
+        <v>8753</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3">
+      <c r="A107" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="C107" s="2">
         <v>8753</v>
       </c>
     </row>

</xml_diff>